<commit_message>
create a file enu,
</commit_message>
<xml_diff>
--- a/res/N4_Kanji_List.xlsx
+++ b/res/N4_Kanji_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProGramming_Projects\Python\KanjiBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProGramming_Projects\Python\KanjiBot\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC5E00A8-C6E9-4441-A1C7-18D2D537F642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63384B9-1E82-4819-A3E4-42FED0A252AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -3155,7 +3155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3512,7 +3512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>

<commit_message>
fixed the sending only 5 kani bug
</commit_message>
<xml_diff>
--- a/res/N4_Kanji_List.xlsx
+++ b/res/N4_Kanji_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProGramming_Projects\Python\KanjiBot\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63384B9-1E82-4819-A3E4-42FED0A252AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DFD20B-5E16-49EF-96E5-9E50DBCE4BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3516,10 +3516,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C444"/>
+  <dimension ref="A1:D363"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A389" workbookViewId="0">
+      <selection activeCell="A412" sqref="A332:XFD412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3528,11 +3528,11 @@
     <col min="2" max="2" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>317</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3564,8 +3564,9 @@
       <c r="C4" s="3" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3575,8 +3576,9 @@
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -3586,8 +3588,9 @@
       <c r="C6" s="3" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -3597,8 +3600,9 @@
       <c r="C7" s="3" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -3608,8 +3612,9 @@
       <c r="C8" s="3" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3619,8 +3624,9 @@
       <c r="C9" s="3" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -3630,8 +3636,9 @@
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -3641,8 +3648,9 @@
       <c r="C11" s="3" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -3652,8 +3660,9 @@
       <c r="C12" s="3" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -3663,8 +3672,9 @@
       <c r="C13" s="3" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -3674,8 +3684,9 @@
       <c r="C14" s="3" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -3685,8 +3696,9 @@
       <c r="C15" s="3" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -3696,8 +3708,9 @@
       <c r="C16" s="3" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -3707,8 +3720,9 @@
       <c r="C17" s="3" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -3718,8 +3732,9 @@
       <c r="C18" s="3" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -3729,8 +3744,9 @@
       <c r="C19" s="3" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -3740,8 +3756,9 @@
       <c r="C20" s="3" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -3751,8 +3768,9 @@
       <c r="C21" s="3" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -3762,8 +3780,9 @@
       <c r="C22" s="3" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -3773,8 +3792,9 @@
       <c r="C23" s="3" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -3784,8 +3804,9 @@
       <c r="C24" s="3" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -3795,8 +3816,9 @@
       <c r="C25" s="3" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -3806,8 +3828,9 @@
       <c r="C26" s="3" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -3817,8 +3840,9 @@
       <c r="C27" s="3" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -3828,8 +3852,9 @@
       <c r="C28" s="3" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -3839,8 +3864,9 @@
       <c r="C29" s="3" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -3850,8 +3876,9 @@
       <c r="C30" s="3" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -3861,8 +3888,9 @@
       <c r="C31" s="3" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -3872,8 +3900,9 @@
       <c r="C32" s="3" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -3883,8 +3912,9 @@
       <c r="C33" s="3" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -3894,8 +3924,9 @@
       <c r="C34" s="3" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -3905,8 +3936,9 @@
       <c r="C35" s="3" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -3916,8 +3948,9 @@
       <c r="C36" s="3" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -3927,8 +3960,9 @@
       <c r="C37" s="3" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -3938,8 +3972,9 @@
       <c r="C38" s="3" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -3949,8 +3984,9 @@
       <c r="C39" s="3" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -3960,8 +3996,9 @@
       <c r="C40" s="3" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -3971,8 +4008,9 @@
       <c r="C41" s="3" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -3982,8 +4020,9 @@
       <c r="C42" s="3" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -3993,8 +4032,9 @@
       <c r="C43" s="3" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -4004,8 +4044,9 @@
       <c r="C44" s="3" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -4015,8 +4056,9 @@
       <c r="C45" s="3" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
@@ -4026,8 +4068,9 @@
       <c r="C46" s="3" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
@@ -4037,8 +4080,9 @@
       <c r="C47" s="3" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -4048,8 +4092,9 @@
       <c r="C48" s="3" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
@@ -4059,8 +4104,9 @@
       <c r="C49" s="3" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
@@ -4070,8 +4116,9 @@
       <c r="C50" s="3" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
@@ -4081,8 +4128,9 @@
       <c r="C51" s="3" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
@@ -4092,8 +4140,9 @@
       <c r="C52" s="3" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
@@ -4103,8 +4152,9 @@
       <c r="C53" s="3" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
@@ -4114,8 +4164,9 @@
       <c r="C54" s="3" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>51</v>
       </c>
@@ -4125,8 +4176,9 @@
       <c r="C55" s="3" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
@@ -4136,8 +4188,9 @@
       <c r="C56" s="3" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
@@ -4147,8 +4200,9 @@
       <c r="C57" s="3" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>54</v>
       </c>
@@ -4158,8 +4212,9 @@
       <c r="C58" s="3" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>55</v>
       </c>
@@ -4169,8 +4224,9 @@
       <c r="C59" s="3" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>56</v>
       </c>
@@ -4180,8 +4236,9 @@
       <c r="C60" s="3" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>57</v>
       </c>
@@ -4191,8 +4248,9 @@
       <c r="C61" s="3" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>58</v>
       </c>
@@ -4202,8 +4260,9 @@
       <c r="C62" s="3" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>59</v>
       </c>
@@ -4213,8 +4272,9 @@
       <c r="C63" s="3" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>60</v>
       </c>
@@ -4224,8 +4284,9 @@
       <c r="C64" s="3" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>61</v>
       </c>
@@ -4235,8 +4296,9 @@
       <c r="C65" s="3" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>62</v>
       </c>
@@ -4246,8 +4308,9 @@
       <c r="C66" s="3" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>63</v>
       </c>
@@ -4257,8 +4320,9 @@
       <c r="C67" s="3" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>64</v>
       </c>
@@ -4268,8 +4332,9 @@
       <c r="C68" s="3" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
@@ -4279,8 +4344,9 @@
       <c r="C69" s="3" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>66</v>
       </c>
@@ -4290,8 +4356,9 @@
       <c r="C70" s="3" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>67</v>
       </c>
@@ -4301,8 +4368,9 @@
       <c r="C71" s="3" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>68</v>
       </c>
@@ -4312,8 +4380,9 @@
       <c r="C72" s="3" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>69</v>
       </c>
@@ -4323,8 +4392,9 @@
       <c r="C73" s="3" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>70</v>
       </c>
@@ -4334,8 +4404,9 @@
       <c r="C74" s="3" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>71</v>
       </c>
@@ -4345,8 +4416,9 @@
       <c r="C75" s="3" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>72</v>
       </c>
@@ -4356,8 +4428,9 @@
       <c r="C76" s="3" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>73</v>
       </c>
@@ -4367,8 +4440,9 @@
       <c r="C77" s="3" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="3"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>74</v>
       </c>
@@ -4378,8 +4452,9 @@
       <c r="C78" s="3" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>75</v>
       </c>
@@ -4389,8 +4464,9 @@
       <c r="C79" s="3" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>76</v>
       </c>
@@ -4400,8 +4476,9 @@
       <c r="C80" s="3" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>77</v>
       </c>
@@ -4411,8 +4488,9 @@
       <c r="C81" s="3" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>78</v>
       </c>
@@ -4422,8 +4500,9 @@
       <c r="C82" s="3" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="3"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>79</v>
       </c>
@@ -4433,8 +4512,9 @@
       <c r="C83" s="3" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>80</v>
       </c>
@@ -4444,8 +4524,9 @@
       <c r="C84" s="3" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="3"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>81</v>
       </c>
@@ -4455,8 +4536,9 @@
       <c r="C85" s="3" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>82</v>
       </c>
@@ -4466,8 +4548,9 @@
       <c r="C86" s="3" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>83</v>
       </c>
@@ -4477,8 +4560,9 @@
       <c r="C87" s="3" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>84</v>
       </c>
@@ -4488,8 +4572,9 @@
       <c r="C88" s="3" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -4499,8 +4584,9 @@
       <c r="C89" s="3" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="3"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>86</v>
       </c>
@@ -4510,8 +4596,9 @@
       <c r="C90" s="3" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="3"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>87</v>
       </c>
@@ -4521,8 +4608,9 @@
       <c r="C91" s="3" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>88</v>
       </c>
@@ -4532,8 +4620,9 @@
       <c r="C92" s="3" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="3"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>89</v>
       </c>
@@ -4543,8 +4632,9 @@
       <c r="C93" s="3" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>90</v>
       </c>
@@ -4554,8 +4644,9 @@
       <c r="C94" s="3" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="3"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>91</v>
       </c>
@@ -4565,8 +4656,9 @@
       <c r="C95" s="3" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>92</v>
       </c>
@@ -4576,8 +4668,9 @@
       <c r="C96" s="3" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="3"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>93</v>
       </c>
@@ -4587,8 +4680,9 @@
       <c r="C97" s="3" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>94</v>
       </c>
@@ -4598,8 +4692,9 @@
       <c r="C98" s="3" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="3"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>95</v>
       </c>
@@ -4609,8 +4704,9 @@
       <c r="C99" s="3" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" s="3"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>96</v>
       </c>
@@ -4620,8 +4716,9 @@
       <c r="C100" s="3" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" s="3"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>97</v>
       </c>
@@ -4631,8 +4728,9 @@
       <c r="C101" s="3" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" s="3"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>98</v>
       </c>
@@ -4642,8 +4740,9 @@
       <c r="C102" s="3" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" s="3"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>99</v>
       </c>
@@ -4653,8 +4752,9 @@
       <c r="C103" s="3" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>100</v>
       </c>
@@ -4664,8 +4764,9 @@
       <c r="C104" s="3" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="3"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>101</v>
       </c>
@@ -4675,8 +4776,9 @@
       <c r="C105" s="3" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>102</v>
       </c>
@@ -4686,8 +4788,9 @@
       <c r="C106" s="3" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" s="3"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>103</v>
       </c>
@@ -4697,8 +4800,9 @@
       <c r="C107" s="3" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" s="3"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>104</v>
       </c>
@@ -4708,8 +4812,9 @@
       <c r="C108" s="3" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="3"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>105</v>
       </c>
@@ -4719,8 +4824,9 @@
       <c r="C109" s="3" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" s="3"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>106</v>
       </c>
@@ -4730,8 +4836,9 @@
       <c r="C110" s="3" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" s="3"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>107</v>
       </c>
@@ -4741,8 +4848,9 @@
       <c r="C111" s="3" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" s="3"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>108</v>
       </c>
@@ -4752,8 +4860,9 @@
       <c r="C112" s="3" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" s="3"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>108</v>
       </c>
@@ -4763,8 +4872,9 @@
       <c r="C113" s="3" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" s="3"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>109</v>
       </c>
@@ -4774,8 +4884,9 @@
       <c r="C114" s="3" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" s="3"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>110</v>
       </c>
@@ -4785,8 +4896,9 @@
       <c r="C115" s="3" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" s="3"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>110</v>
       </c>
@@ -4796,8 +4908,9 @@
       <c r="C116" s="3" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" s="3"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>111</v>
       </c>
@@ -4807,8 +4920,9 @@
       <c r="C117" s="3" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" s="3"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>112</v>
       </c>
@@ -4818,8 +4932,9 @@
       <c r="C118" s="3" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118" s="3"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>113</v>
       </c>
@@ -4829,8 +4944,9 @@
       <c r="C119" s="3" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" s="3"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>114</v>
       </c>
@@ -4840,8 +4956,9 @@
       <c r="C120" s="3" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120" s="3"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>115</v>
       </c>
@@ -4851,8 +4968,9 @@
       <c r="C121" s="3" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>116</v>
       </c>
@@ -4862,8 +4980,9 @@
       <c r="C122" s="3" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122" s="3"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>117</v>
       </c>
@@ -4873,8 +4992,9 @@
       <c r="C123" s="3" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" s="3"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>118</v>
       </c>
@@ -4884,8 +5004,9 @@
       <c r="C124" s="3" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124" s="3"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>119</v>
       </c>
@@ -4895,8 +5016,9 @@
       <c r="C125" s="3" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125" s="3"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>120</v>
       </c>
@@ -4906,8 +5028,9 @@
       <c r="C126" s="3" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126" s="3"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>121</v>
       </c>
@@ -4917,8 +5040,9 @@
       <c r="C127" s="3" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127" s="3"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>122</v>
       </c>
@@ -4928,8 +5052,9 @@
       <c r="C128" s="3" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>123</v>
       </c>
@@ -4939,8 +5064,9 @@
       <c r="C129" s="3" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129" s="3"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>124</v>
       </c>
@@ -4950,8 +5076,9 @@
       <c r="C130" s="3" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130" s="3"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>125</v>
       </c>
@@ -4961,8 +5088,9 @@
       <c r="C131" s="3" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131" s="3"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>126</v>
       </c>
@@ -4972,8 +5100,9 @@
       <c r="C132" s="3" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132" s="3"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>127</v>
       </c>
@@ -4983,8 +5112,9 @@
       <c r="C133" s="3" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133" s="3"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>128</v>
       </c>
@@ -4994,8 +5124,9 @@
       <c r="C134" s="3" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134" s="3"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>129</v>
       </c>
@@ -5005,8 +5136,9 @@
       <c r="C135" s="3" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135" s="3"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>130</v>
       </c>
@@ -5016,8 +5148,9 @@
       <c r="C136" s="3" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136" s="3"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>130</v>
       </c>
@@ -5027,8 +5160,9 @@
       <c r="C137" s="3" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137" s="3"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>131</v>
       </c>
@@ -5038,8 +5172,9 @@
       <c r="C138" s="3" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138" s="3"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>131</v>
       </c>
@@ -5049,8 +5184,9 @@
       <c r="C139" s="3" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139" s="3"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>132</v>
       </c>
@@ -5060,8 +5196,9 @@
       <c r="C140" s="3" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140" s="3"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>133</v>
       </c>
@@ -5071,8 +5208,9 @@
       <c r="C141" s="3" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" s="3"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>134</v>
       </c>
@@ -5082,8 +5220,9 @@
       <c r="C142" s="3" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" s="3"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>135</v>
       </c>
@@ -5093,8 +5232,9 @@
       <c r="C143" s="3" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143" s="3"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>136</v>
       </c>
@@ -5104,8 +5244,9 @@
       <c r="C144" s="3" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144" s="3"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>137</v>
       </c>
@@ -5115,8 +5256,9 @@
       <c r="C145" s="3" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145" s="3"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>138</v>
       </c>
@@ -5126,8 +5268,9 @@
       <c r="C146" s="3" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146" s="3"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>139</v>
       </c>
@@ -5137,8 +5280,9 @@
       <c r="C147" s="3" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147" s="3"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>140</v>
       </c>
@@ -5148,8 +5292,9 @@
       <c r="C148" s="3" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148" s="3"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>141</v>
       </c>
@@ -5159,8 +5304,9 @@
       <c r="C149" s="3" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149" s="3"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>142</v>
       </c>
@@ -5170,8 +5316,9 @@
       <c r="C150" s="3" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150" s="3"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>143</v>
       </c>
@@ -5181,8 +5328,9 @@
       <c r="C151" s="3" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" s="3"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>144</v>
       </c>
@@ -5192,8 +5340,9 @@
       <c r="C152" s="3" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" s="3"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>145</v>
       </c>
@@ -5203,8 +5352,9 @@
       <c r="C153" s="3" t="s">
         <v>763</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" s="3"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>146</v>
       </c>
@@ -5214,8 +5364,9 @@
       <c r="C154" s="3" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154" s="3"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>147</v>
       </c>
@@ -5225,8 +5376,9 @@
       <c r="C155" s="3" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155" s="3"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>148</v>
       </c>
@@ -5236,8 +5388,9 @@
       <c r="C156" s="3" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156" s="3"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>149</v>
       </c>
@@ -5247,8 +5400,9 @@
       <c r="C157" s="3" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157" s="3"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>150</v>
       </c>
@@ -5258,8 +5412,9 @@
       <c r="C158" s="3" t="s">
         <v>768</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158" s="3"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>151</v>
       </c>
@@ -5269,8 +5424,9 @@
       <c r="C159" s="3" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159" s="3"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>152</v>
       </c>
@@ -5280,8 +5436,9 @@
       <c r="C160" s="3" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160" s="3"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>152</v>
       </c>
@@ -5291,8 +5448,9 @@
       <c r="C161" s="3" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161" s="3"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>153</v>
       </c>
@@ -5302,8 +5460,9 @@
       <c r="C162" s="3" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162" s="3"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>154</v>
       </c>
@@ -5313,8 +5472,9 @@
       <c r="C163" s="3" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163" s="3"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>155</v>
       </c>
@@ -5324,8 +5484,9 @@
       <c r="C164" s="3" t="s">
         <v>774</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164" s="3"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>156</v>
       </c>
@@ -5335,8 +5496,9 @@
       <c r="C165" s="3" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165" s="3"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>157</v>
       </c>
@@ -5346,8 +5508,9 @@
       <c r="C166" s="3" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166" s="3"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>158</v>
       </c>
@@ -5357,8 +5520,9 @@
       <c r="C167" s="3" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167" s="3"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>159</v>
       </c>
@@ -5368,8 +5532,9 @@
       <c r="C168" s="3" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168" s="3"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>160</v>
       </c>
@@ -5379,8 +5544,9 @@
       <c r="C169" s="3" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169" s="3"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>161</v>
       </c>
@@ -5390,8 +5556,9 @@
       <c r="C170" s="3" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170" s="3"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>162</v>
       </c>
@@ -5401,8 +5568,9 @@
       <c r="C171" s="3" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D171" s="3"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>163</v>
       </c>
@@ -5412,8 +5580,9 @@
       <c r="C172" s="3" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172" s="3"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>164</v>
       </c>
@@ -5423,8 +5592,9 @@
       <c r="C173" s="3" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D173" s="3"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>165</v>
       </c>
@@ -5434,8 +5604,9 @@
       <c r="C174" s="3" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D174" s="3"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>166</v>
       </c>
@@ -5445,8 +5616,9 @@
       <c r="C175" s="3" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D175" s="3"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>167</v>
       </c>
@@ -5456,8 +5628,9 @@
       <c r="C176" s="3" t="s">
         <v>786</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>168</v>
       </c>
@@ -5467,8 +5640,9 @@
       <c r="C177" s="3" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177" s="3"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>169</v>
       </c>
@@ -5478,8 +5652,9 @@
       <c r="C178" s="3" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>169</v>
       </c>
@@ -5489,8 +5664,9 @@
       <c r="C179" s="3" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D179" s="3"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>170</v>
       </c>
@@ -5500,8 +5676,9 @@
       <c r="C180" s="3" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D180" s="3"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>171</v>
       </c>
@@ -5511,8 +5688,9 @@
       <c r="C181" s="3" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D181" s="3"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>172</v>
       </c>
@@ -5522,8 +5700,9 @@
       <c r="C182" s="3" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D182" s="3"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>173</v>
       </c>
@@ -5531,8 +5710,9 @@
       <c r="C183" s="3" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183" s="3"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>174</v>
       </c>
@@ -5542,8 +5722,9 @@
       <c r="C184" s="3" t="s">
         <v>792</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D184" s="3"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>175</v>
       </c>
@@ -5553,8 +5734,9 @@
       <c r="C185" s="3" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185" s="3"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>175</v>
       </c>
@@ -5564,8 +5746,9 @@
       <c r="C186" s="3" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D186" s="3"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>176</v>
       </c>
@@ -5575,8 +5758,9 @@
       <c r="C187" s="3" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D187" s="3"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>177</v>
       </c>
@@ -5586,8 +5770,9 @@
       <c r="C188" s="3" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D188" s="3"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>178</v>
       </c>
@@ -5597,8 +5782,9 @@
       <c r="C189" s="3" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D189" s="3"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>179</v>
       </c>
@@ -5608,8 +5794,9 @@
       <c r="C190" s="3" t="s">
         <v>798</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D190" s="3"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>180</v>
       </c>
@@ -5619,8 +5806,9 @@
       <c r="C191" s="3" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D191" s="3"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>181</v>
       </c>
@@ -5630,8 +5818,9 @@
       <c r="C192" s="3" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D192" s="3"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>182</v>
       </c>
@@ -5641,8 +5830,9 @@
       <c r="C193" s="3" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D193" s="3"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>183</v>
       </c>
@@ -5652,8 +5842,9 @@
       <c r="C194" s="3" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D194" s="3"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>184</v>
       </c>
@@ -5663,8 +5854,9 @@
       <c r="C195" s="3" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D195" s="3"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>185</v>
       </c>
@@ -5674,8 +5866,9 @@
       <c r="C196" s="3" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D196" s="3"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>186</v>
       </c>
@@ -5685,8 +5878,9 @@
       <c r="C197" s="3" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D197" s="3"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>187</v>
       </c>
@@ -5696,8 +5890,9 @@
       <c r="C198" s="3" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D198" s="3"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>188</v>
       </c>
@@ -5707,8 +5902,9 @@
       <c r="C199" s="3" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D199" s="3"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>189</v>
       </c>
@@ -5718,8 +5914,9 @@
       <c r="C200" s="3" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D200" s="3"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>190</v>
       </c>
@@ -5729,8 +5926,9 @@
       <c r="C201" s="3" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D201" s="3"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>191</v>
       </c>
@@ -5740,8 +5938,9 @@
       <c r="C202" s="3" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D202" s="3"/>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>192</v>
       </c>
@@ -5751,8 +5950,9 @@
       <c r="C203" s="3" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D203" s="3"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>193</v>
       </c>
@@ -5762,8 +5962,9 @@
       <c r="C204" s="3" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D204" s="3"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>194</v>
       </c>
@@ -5773,8 +5974,9 @@
       <c r="C205" s="3" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D205" s="3"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>195</v>
       </c>
@@ -5784,8 +5986,9 @@
       <c r="C206" s="3" t="s">
         <v>814</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>196</v>
       </c>
@@ -5795,8 +5998,9 @@
       <c r="C207" s="3" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D207" s="3"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>197</v>
       </c>
@@ -5806,8 +6010,9 @@
       <c r="C208" s="3" t="s">
         <v>816</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D208" s="3"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>198</v>
       </c>
@@ -5817,8 +6022,9 @@
       <c r="C209" s="3" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D209" s="3"/>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>199</v>
       </c>
@@ -5828,8 +6034,9 @@
       <c r="C210" s="3" t="s">
         <v>818</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D210" s="3"/>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>200</v>
       </c>
@@ -5839,8 +6046,9 @@
       <c r="C211" s="3" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D211" s="3"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>201</v>
       </c>
@@ -5850,8 +6058,9 @@
       <c r="C212" s="3" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D212" s="3"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>202</v>
       </c>
@@ -5861,8 +6070,9 @@
       <c r="C213" s="3" t="s">
         <v>821</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D213" s="3"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>203</v>
       </c>
@@ -5872,8 +6082,9 @@
       <c r="C214" s="3" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D214" s="3"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>204</v>
       </c>
@@ -5883,8 +6094,9 @@
       <c r="C215" s="3" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D215" s="3"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>205</v>
       </c>
@@ -5894,8 +6106,9 @@
       <c r="C216" s="3" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D216" s="3"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>206</v>
       </c>
@@ -5905,8 +6118,9 @@
       <c r="C217" s="3" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D217" s="3"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>207</v>
       </c>
@@ -5916,8 +6130,9 @@
       <c r="C218" s="3" t="s">
         <v>826</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D218" s="3"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>208</v>
       </c>
@@ -5927,8 +6142,9 @@
       <c r="C219" s="3" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D219" s="3"/>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>209</v>
       </c>
@@ -5938,8 +6154,9 @@
       <c r="C220" s="3" t="s">
         <v>828</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D220" s="3"/>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>210</v>
       </c>
@@ -5949,8 +6166,9 @@
       <c r="C221" s="3" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D221" s="3"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>211</v>
       </c>
@@ -5960,8 +6178,9 @@
       <c r="C222" s="3" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D222" s="3"/>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>212</v>
       </c>
@@ -5971,8 +6190,9 @@
       <c r="C223" s="3" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D223" s="3"/>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>213</v>
       </c>
@@ -5982,8 +6202,9 @@
       <c r="C224" s="3" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D224" s="3"/>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>214</v>
       </c>
@@ -5993,8 +6214,9 @@
       <c r="C225" s="3" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D225" s="3"/>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>215</v>
       </c>
@@ -6004,8 +6226,9 @@
       <c r="C226" s="3" t="s">
         <v>833</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D226" s="3"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>216</v>
       </c>
@@ -6015,8 +6238,9 @@
       <c r="C227" s="3" t="s">
         <v>834</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D227" s="3"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>217</v>
       </c>
@@ -6026,8 +6250,9 @@
       <c r="C228" s="3" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D228" s="3"/>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>218</v>
       </c>
@@ -6037,8 +6262,9 @@
       <c r="C229" s="3" t="s">
         <v>836</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D229" s="3"/>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>219</v>
       </c>
@@ -6048,8 +6274,9 @@
       <c r="C230" s="3" t="s">
         <v>837</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D230" s="3"/>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>220</v>
       </c>
@@ -6059,8 +6286,9 @@
       <c r="C231" s="3" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D231" s="3"/>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>221</v>
       </c>
@@ -6070,8 +6298,9 @@
       <c r="C232" s="3" t="s">
         <v>839</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D232" s="3"/>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>222</v>
       </c>
@@ -6081,8 +6310,9 @@
       <c r="C233" s="3" t="s">
         <v>840</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D233" s="3"/>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>223</v>
       </c>
@@ -6092,8 +6322,9 @@
       <c r="C234" s="3" t="s">
         <v>841</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D234" s="3"/>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>224</v>
       </c>
@@ -6103,8 +6334,9 @@
       <c r="C235" s="3" t="s">
         <v>842</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D235" s="3"/>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>225</v>
       </c>
@@ -6114,8 +6346,9 @@
       <c r="C236" s="3" t="s">
         <v>843</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D236" s="3"/>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>226</v>
       </c>
@@ -6125,8 +6358,9 @@
       <c r="C237" s="3" t="s">
         <v>844</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D237" s="3"/>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>227</v>
       </c>
@@ -6136,8 +6370,9 @@
       <c r="C238" s="3" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D238" s="3"/>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>228</v>
       </c>
@@ -6147,8 +6382,9 @@
       <c r="C239" s="3" t="s">
         <v>846</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D239" s="3"/>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>229</v>
       </c>
@@ -6158,8 +6394,9 @@
       <c r="C240" s="3" t="s">
         <v>847</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D240" s="3"/>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>230</v>
       </c>
@@ -6169,8 +6406,9 @@
       <c r="C241" s="3" t="s">
         <v>848</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D241" s="3"/>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>231</v>
       </c>
@@ -6180,8 +6418,9 @@
       <c r="C242" s="3" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D242" s="3"/>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>232</v>
       </c>
@@ -6191,8 +6430,9 @@
       <c r="C243" s="3" t="s">
         <v>850</v>
       </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D243" s="3"/>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>233</v>
       </c>
@@ -6202,8 +6442,9 @@
       <c r="C244" s="3" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D244" s="3"/>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>234</v>
       </c>
@@ -6211,8 +6452,9 @@
       <c r="C245" s="3" t="s">
         <v>852</v>
       </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D245" s="3"/>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>235</v>
       </c>
@@ -6222,8 +6464,9 @@
       <c r="C246" s="3" t="s">
         <v>853</v>
       </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D246" s="3"/>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>236</v>
       </c>
@@ -6233,8 +6476,9 @@
       <c r="C247" s="3" t="s">
         <v>854</v>
       </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D247" s="3"/>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>237</v>
       </c>
@@ -6244,8 +6488,9 @@
       <c r="C248" s="3" t="s">
         <v>855</v>
       </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D248" s="3"/>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>238</v>
       </c>
@@ -6255,8 +6500,9 @@
       <c r="C249" s="3" t="s">
         <v>856</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D249" s="3"/>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>239</v>
       </c>
@@ -6266,8 +6512,9 @@
       <c r="C250" s="3" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D250" s="3"/>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>240</v>
       </c>
@@ -6277,8 +6524,9 @@
       <c r="C251" s="3" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D251" s="3"/>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>241</v>
       </c>
@@ -6288,8 +6536,9 @@
       <c r="C252" s="3" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D252" s="3"/>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>242</v>
       </c>
@@ -6299,8 +6548,9 @@
       <c r="C253" s="3" t="s">
         <v>860</v>
       </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D253" s="3"/>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>243</v>
       </c>
@@ -6310,8 +6560,9 @@
       <c r="C254" s="3" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D254" s="3"/>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>244</v>
       </c>
@@ -6321,8 +6572,9 @@
       <c r="C255" s="3" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D255" s="3"/>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>245</v>
       </c>
@@ -6332,8 +6584,9 @@
       <c r="C256" s="3" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D256" s="3"/>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>246</v>
       </c>
@@ -6343,8 +6596,9 @@
       <c r="C257" s="3" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D257" s="3"/>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>247</v>
       </c>
@@ -6354,8 +6608,9 @@
       <c r="C258" s="3" t="s">
         <v>865</v>
       </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D258" s="3"/>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>248</v>
       </c>
@@ -6365,8 +6620,9 @@
       <c r="C259" s="3" t="s">
         <v>866</v>
       </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D259" s="3"/>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>249</v>
       </c>
@@ -6376,8 +6632,9 @@
       <c r="C260" s="3" t="s">
         <v>867</v>
       </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D260" s="3"/>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>250</v>
       </c>
@@ -6387,8 +6644,9 @@
       <c r="C261" s="3" t="s">
         <v>868</v>
       </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D261" s="3"/>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>251</v>
       </c>
@@ -6398,8 +6656,9 @@
       <c r="C262" s="3" t="s">
         <v>869</v>
       </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D262" s="3"/>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>252</v>
       </c>
@@ -6409,8 +6668,9 @@
       <c r="C263" s="3" t="s">
         <v>870</v>
       </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D263" s="3"/>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>253</v>
       </c>
@@ -6420,8 +6680,9 @@
       <c r="C264" s="3" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D264" s="3"/>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>254</v>
       </c>
@@ -6431,8 +6692,9 @@
       <c r="C265" s="3" t="s">
         <v>872</v>
       </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D265" s="3"/>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>255</v>
       </c>
@@ -6442,8 +6704,9 @@
       <c r="C266" s="3" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D266" s="3"/>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>256</v>
       </c>
@@ -6453,8 +6716,9 @@
       <c r="C267" s="3" t="s">
         <v>874</v>
       </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D267" s="3"/>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>257</v>
       </c>
@@ -6464,8 +6728,9 @@
       <c r="C268" s="3" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D268" s="3"/>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>258</v>
       </c>
@@ -6475,8 +6740,9 @@
       <c r="C269" s="3" t="s">
         <v>876</v>
       </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D269" s="3"/>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>259</v>
       </c>
@@ -6486,8 +6752,9 @@
       <c r="C270" s="3" t="s">
         <v>877</v>
       </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D270" s="3"/>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>260</v>
       </c>
@@ -6497,8 +6764,9 @@
       <c r="C271" s="3" t="s">
         <v>878</v>
       </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D271" s="3"/>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>261</v>
       </c>
@@ -6508,8 +6776,9 @@
       <c r="C272" s="3" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D272" s="3"/>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>262</v>
       </c>
@@ -6519,8 +6788,9 @@
       <c r="C273" s="3" t="s">
         <v>880</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D273" s="3"/>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>263</v>
       </c>
@@ -6530,8 +6800,9 @@
       <c r="C274" s="3" t="s">
         <v>881</v>
       </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D274" s="3"/>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>263</v>
       </c>
@@ -6541,8 +6812,9 @@
       <c r="C275" s="3" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D275" s="3"/>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>264</v>
       </c>
@@ -6552,8 +6824,9 @@
       <c r="C276" s="3" t="s">
         <v>883</v>
       </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D276" s="3"/>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>265</v>
       </c>
@@ -6563,8 +6836,9 @@
       <c r="C277" s="3" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D277" s="3"/>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>266</v>
       </c>
@@ -6574,8 +6848,9 @@
       <c r="C278" s="3" t="s">
         <v>884</v>
       </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D278" s="3"/>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>267</v>
       </c>
@@ -6585,8 +6860,9 @@
       <c r="C279" s="3" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D279" s="3"/>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>268</v>
       </c>
@@ -6596,8 +6872,9 @@
       <c r="C280" s="3" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D280" s="3"/>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>269</v>
       </c>
@@ -6607,8 +6884,9 @@
       <c r="C281" s="3" t="s">
         <v>887</v>
       </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D281" s="3"/>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>270</v>
       </c>
@@ -6618,8 +6896,9 @@
       <c r="C282" s="3" t="s">
         <v>888</v>
       </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D282" s="3"/>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>271</v>
       </c>
@@ -6629,8 +6908,9 @@
       <c r="C283" s="3" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D283" s="3"/>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>272</v>
       </c>
@@ -6640,8 +6920,9 @@
       <c r="C284" s="3" t="s">
         <v>890</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D284" s="3"/>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>273</v>
       </c>
@@ -6651,8 +6932,9 @@
       <c r="C285" s="3" t="s">
         <v>891</v>
       </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D285" s="3"/>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>274</v>
       </c>
@@ -6662,8 +6944,9 @@
       <c r="C286" s="3" t="s">
         <v>892</v>
       </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D286" s="3"/>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>275</v>
       </c>
@@ -6673,8 +6956,9 @@
       <c r="C287" s="3" t="s">
         <v>893</v>
       </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D287" s="3"/>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>276</v>
       </c>
@@ -6684,8 +6968,9 @@
       <c r="C288" s="3" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D288" s="3"/>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>277</v>
       </c>
@@ -6695,8 +6980,9 @@
       <c r="C289" s="3" t="s">
         <v>895</v>
       </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D289" s="3"/>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>278</v>
       </c>
@@ -6706,8 +6992,9 @@
       <c r="C290" s="3" t="s">
         <v>896</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D290" s="3"/>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>279</v>
       </c>
@@ -6717,8 +7004,9 @@
       <c r="C291" s="3" t="s">
         <v>897</v>
       </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D291" s="3"/>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>280</v>
       </c>
@@ -6728,8 +7016,9 @@
       <c r="C292" s="3" t="s">
         <v>898</v>
       </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D292" s="3"/>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>281</v>
       </c>
@@ -6739,8 +7028,9 @@
       <c r="C293" s="3" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D293" s="3"/>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>282</v>
       </c>
@@ -6750,8 +7040,9 @@
       <c r="C294" s="3" t="s">
         <v>900</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D294" s="3"/>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>283</v>
       </c>
@@ -6761,8 +7052,9 @@
       <c r="C295" s="3" t="s">
         <v>901</v>
       </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D295" s="3"/>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>283</v>
       </c>
@@ -6772,8 +7064,9 @@
       <c r="C296" s="3" t="s">
         <v>901</v>
       </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D296" s="3"/>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>284</v>
       </c>
@@ -6783,8 +7076,9 @@
       <c r="C297" s="3" t="s">
         <v>902</v>
       </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D297" s="3"/>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>285</v>
       </c>
@@ -6794,8 +7088,9 @@
       <c r="C298" s="3" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D298" s="3"/>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>286</v>
       </c>
@@ -6805,8 +7100,9 @@
       <c r="C299" s="3" t="s">
         <v>904</v>
       </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D299" s="3"/>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>287</v>
       </c>
@@ -6816,8 +7112,9 @@
       <c r="C300" s="3" t="s">
         <v>905</v>
       </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D300" s="3"/>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>288</v>
       </c>
@@ -6827,8 +7124,9 @@
       <c r="C301" s="3" t="s">
         <v>906</v>
       </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D301" s="3"/>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>289</v>
       </c>
@@ -6838,8 +7136,9 @@
       <c r="C302" s="3" t="s">
         <v>907</v>
       </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D302" s="3"/>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>290</v>
       </c>
@@ -6849,8 +7148,9 @@
       <c r="C303" s="3" t="s">
         <v>908</v>
       </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D303" s="3"/>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>291</v>
       </c>
@@ -6860,8 +7160,9 @@
       <c r="C304" s="3" t="s">
         <v>909</v>
       </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D304" s="3"/>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>291</v>
       </c>
@@ -6871,8 +7172,9 @@
       <c r="C305" s="3" t="s">
         <v>910</v>
       </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D305" s="3"/>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>291</v>
       </c>
@@ -6882,8 +7184,9 @@
       <c r="C306" s="3" t="s">
         <v>910</v>
       </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D306" s="3"/>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>292</v>
       </c>
@@ -6893,8 +7196,9 @@
       <c r="C307" s="3" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D307" s="3"/>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>293</v>
       </c>
@@ -6904,8 +7208,9 @@
       <c r="C308" s="3" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D308" s="3"/>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>294</v>
       </c>
@@ -6915,8 +7220,9 @@
       <c r="C309" s="3" t="s">
         <v>913</v>
       </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D309" s="3"/>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>295</v>
       </c>
@@ -6926,8 +7232,9 @@
       <c r="C310" s="3" t="s">
         <v>914</v>
       </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D310" s="3"/>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>296</v>
       </c>
@@ -6937,8 +7244,9 @@
       <c r="C311" s="3" t="s">
         <v>915</v>
       </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D311" s="3"/>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>297</v>
       </c>
@@ -6948,8 +7256,9 @@
       <c r="C312" s="3" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D312" s="3"/>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>298</v>
       </c>
@@ -6959,8 +7268,9 @@
       <c r="C313" s="3" t="s">
         <v>917</v>
       </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D313" s="3"/>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>299</v>
       </c>
@@ -6970,8 +7280,9 @@
       <c r="C314" s="3" t="s">
         <v>918</v>
       </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D314" s="3"/>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>300</v>
       </c>
@@ -6981,8 +7292,9 @@
       <c r="C315" s="3" t="s">
         <v>919</v>
       </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D315" s="3"/>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>301</v>
       </c>
@@ -6992,8 +7304,9 @@
       <c r="C316" s="3" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D316" s="3"/>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>302</v>
       </c>
@@ -7003,8 +7316,9 @@
       <c r="C317" s="3" t="s">
         <v>921</v>
       </c>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D317" s="3"/>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>303</v>
       </c>
@@ -7014,8 +7328,9 @@
       <c r="C318" s="3" t="s">
         <v>922</v>
       </c>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D318" s="3"/>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>304</v>
       </c>
@@ -7025,8 +7340,9 @@
       <c r="C319" s="3" t="s">
         <v>923</v>
       </c>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D319" s="3"/>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>305</v>
       </c>
@@ -7036,8 +7352,9 @@
       <c r="C320" s="3" t="s">
         <v>924</v>
       </c>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D320" s="3"/>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>306</v>
       </c>
@@ -7047,8 +7364,9 @@
       <c r="C321" s="3" t="s">
         <v>925</v>
       </c>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D321" s="3"/>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>307</v>
       </c>
@@ -7058,8 +7376,9 @@
       <c r="C322" s="3" t="s">
         <v>926</v>
       </c>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D322" s="3"/>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>308</v>
       </c>
@@ -7069,8 +7388,9 @@
       <c r="C323" s="3" t="s">
         <v>927</v>
       </c>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D323" s="3"/>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>309</v>
       </c>
@@ -7080,8 +7400,9 @@
       <c r="C324" s="3" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D324" s="3"/>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>310</v>
       </c>
@@ -7091,8 +7412,9 @@
       <c r="C325" s="3" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D325" s="3"/>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>311</v>
       </c>
@@ -7102,8 +7424,9 @@
       <c r="C326" s="3" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D326" s="3"/>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>312</v>
       </c>
@@ -7113,8 +7436,9 @@
       <c r="C327" s="3" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D327" s="3"/>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>313</v>
       </c>
@@ -7124,8 +7448,9 @@
       <c r="C328" s="3" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D328" s="3"/>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>314</v>
       </c>
@@ -7135,8 +7460,9 @@
       <c r="C329" s="3" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D329" s="3"/>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>315</v>
       </c>
@@ -7146,8 +7472,9 @@
       <c r="C330" s="3" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D330" s="3"/>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>316</v>
       </c>
@@ -7157,24 +7484,25 @@
       <c r="C331" s="3" t="s">
         <v>935</v>
       </c>
-    </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D331" s="3"/>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" s="1"/>
       <c r="B332" s="3"/>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" s="1"/>
       <c r="B333" s="3"/>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" s="1"/>
       <c r="B334" s="3"/>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" s="1"/>
       <c r="B335" s="3"/>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" s="1"/>
       <c r="B336" s="3"/>
     </row>
@@ -7263,346 +7591,22 @@
       <c r="B357" s="3"/>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A358" s="1"/>
       <c r="B358" s="3"/>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A359" s="1"/>
       <c r="B359" s="3"/>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A360" s="1"/>
       <c r="B360" s="3"/>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A361" s="1"/>
       <c r="B361" s="3"/>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A362" s="1"/>
       <c r="B362" s="3"/>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A363" s="1"/>
       <c r="B363" s="3"/>
-    </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A364" s="1"/>
-      <c r="B364" s="3"/>
-    </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A365" s="1"/>
-      <c r="B365" s="3"/>
-    </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A366" s="1"/>
-      <c r="B366" s="3"/>
-    </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A367" s="1"/>
-      <c r="B367" s="3"/>
-    </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A368" s="1"/>
-      <c r="B368" s="3"/>
-    </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A369" s="1"/>
-      <c r="B369" s="3"/>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A370" s="1"/>
-      <c r="B370" s="3"/>
-    </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A371" s="1"/>
-      <c r="B371" s="3"/>
-    </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A372" s="1"/>
-      <c r="B372" s="3"/>
-    </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A373" s="1"/>
-      <c r="B373" s="3"/>
-    </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A374" s="1"/>
-      <c r="B374" s="3"/>
-    </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A375" s="1"/>
-      <c r="B375" s="3"/>
-    </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A376" s="1"/>
-      <c r="B376" s="3"/>
-    </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A377" s="1"/>
-      <c r="B377" s="3"/>
-    </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A378" s="1"/>
-      <c r="B378" s="3"/>
-    </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A379" s="1"/>
-      <c r="B379" s="3"/>
-    </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A380" s="1"/>
-      <c r="B380" s="3"/>
-    </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A381" s="1"/>
-      <c r="B381" s="3"/>
-    </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A382" s="1"/>
-      <c r="B382" s="3"/>
-    </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A383" s="1"/>
-      <c r="B383" s="3"/>
-    </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A384" s="1"/>
-      <c r="B384" s="3"/>
-    </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A385" s="1"/>
-      <c r="B385" s="3"/>
-    </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A386" s="1"/>
-      <c r="B386" s="3"/>
-    </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A387" s="1"/>
-      <c r="B387" s="3"/>
-    </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A388" s="1"/>
-      <c r="B388" s="3"/>
-    </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A389" s="1"/>
-      <c r="B389" s="3"/>
-    </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A390" s="1"/>
-      <c r="B390" s="3"/>
-    </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A391" s="1"/>
-      <c r="B391" s="3"/>
-    </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A392" s="1"/>
-      <c r="B392" s="3"/>
-    </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A393" s="1"/>
-      <c r="B393" s="3"/>
-    </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A394" s="1"/>
-      <c r="B394" s="3"/>
-    </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A395" s="1"/>
-      <c r="B395" s="3"/>
-    </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A396" s="1"/>
-      <c r="B396" s="3"/>
-    </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A397" s="1"/>
-      <c r="B397" s="3"/>
-    </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A398" s="1"/>
-      <c r="B398" s="3"/>
-    </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A399" s="1"/>
-      <c r="B399" s="3"/>
-    </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A400" s="1"/>
-      <c r="B400" s="3"/>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A401" s="1"/>
-      <c r="B401" s="3"/>
-    </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A402" s="1"/>
-      <c r="B402" s="3"/>
-    </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A403" s="1"/>
-      <c r="B403" s="3"/>
-    </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A404" s="1"/>
-      <c r="B404" s="3"/>
-    </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A405" s="1"/>
-      <c r="B405" s="3"/>
-    </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A406" s="1"/>
-      <c r="B406" s="3"/>
-    </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A407" s="1"/>
-      <c r="B407" s="3"/>
-    </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A408" s="1"/>
-      <c r="B408" s="3"/>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A409" s="1"/>
-      <c r="B409" s="3"/>
-    </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A410" s="1"/>
-      <c r="B410" s="3"/>
-    </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A411" s="1"/>
-      <c r="B411" s="3"/>
-    </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A412" s="1"/>
-      <c r="B412" s="3"/>
-    </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A413" s="1"/>
-      <c r="B413" s="3"/>
-    </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A414" s="1"/>
-      <c r="B414" s="3"/>
-    </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A415" s="1"/>
-      <c r="B415" s="3"/>
-    </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A416" s="1"/>
-      <c r="B416" s="3"/>
-    </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A417" s="1"/>
-      <c r="B417" s="3"/>
-    </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A418" s="1"/>
-      <c r="B418" s="3"/>
-    </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A419" s="1"/>
-      <c r="B419" s="3"/>
-    </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A420" s="1"/>
-      <c r="B420" s="3"/>
-    </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A421" s="1"/>
-      <c r="B421" s="3"/>
-    </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A422" s="1"/>
-      <c r="B422" s="3"/>
-    </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A423" s="1"/>
-      <c r="B423" s="3"/>
-    </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A424" s="1"/>
-      <c r="B424" s="3"/>
-    </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A425" s="1"/>
-      <c r="B425" s="3"/>
-    </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A426" s="1"/>
-      <c r="B426" s="3"/>
-    </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A427" s="1"/>
-      <c r="B427" s="3"/>
-    </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A428" s="1"/>
-      <c r="B428" s="3"/>
-    </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A429" s="1"/>
-      <c r="B429" s="3"/>
-    </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A430" s="1"/>
-      <c r="B430" s="3"/>
-    </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A431" s="1"/>
-      <c r="B431" s="3"/>
-    </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A432" s="1"/>
-      <c r="B432" s="3"/>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A433" s="1"/>
-      <c r="B433" s="3"/>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A434" s="1"/>
-      <c r="B434" s="3"/>
-    </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A435" s="1"/>
-      <c r="B435" s="3"/>
-    </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A436" s="1"/>
-      <c r="B436" s="3"/>
-    </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A437" s="1"/>
-      <c r="B437" s="3"/>
-    </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A438" s="1"/>
-      <c r="B438" s="3"/>
-    </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B439" s="3"/>
-    </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B440" s="3"/>
-    </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B441" s="3"/>
-    </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B442" s="3"/>
-    </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B443" s="3"/>
-    </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B444" s="3"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>